<commit_message>
Resultados tempos finais concluido
</commit_message>
<xml_diff>
--- a/gesthiper.xlsx
+++ b/gesthiper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="82">
   <si>
     <t>Queries</t>
   </si>
@@ -242,6 +242,30 @@
   </si>
   <si>
     <t>0.17 ms</t>
+  </si>
+  <si>
+    <t>2.06 ms</t>
+  </si>
+  <si>
+    <t>59.42 ms</t>
+  </si>
+  <si>
+    <t>0.21 ms</t>
+  </si>
+  <si>
+    <t>0.75 ms</t>
+  </si>
+  <si>
+    <t>1.42 ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.19 ms</t>
+  </si>
+  <si>
+    <t>88.71 ms</t>
+  </si>
+  <si>
+    <t>0.24 ms</t>
   </si>
 </sst>
 </file>
@@ -869,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -942,7 +966,9 @@
       <c r="H2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="4"/>
+      <c r="I2" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="J2" s="4" t="s">
         <v>19</v>
       </c>
@@ -972,7 +998,9 @@
       <c r="H3" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I3" s="4"/>
+      <c r="I3" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="J3" s="4" t="s">
         <v>18</v>
       </c>
@@ -1002,7 +1030,9 @@
       <c r="H4" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="I4" s="4"/>
+      <c r="I4" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="J4" s="4" t="s">
         <v>22</v>
       </c>
@@ -1032,7 +1062,9 @@
       <c r="H5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I5" s="4"/>
+      <c r="I5" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="J5" s="4" t="s">
         <v>19</v>
       </c>
@@ -1062,7 +1094,9 @@
       <c r="H6" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="I6" s="4"/>
+      <c r="I6" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="J6" s="4" t="s">
         <v>19</v>
       </c>
@@ -1092,7 +1126,9 @@
       <c r="H7" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="J7" s="4" t="s">
         <v>18</v>
       </c>
@@ -1122,7 +1158,9 @@
       <c r="H8" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="4"/>
+      <c r="I8" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="J8" s="4" t="s">
         <v>20</v>
       </c>
@@ -1152,7 +1190,9 @@
       <c r="H9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="4"/>
+      <c r="I9" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="J9" s="4" t="s">
         <v>19</v>
       </c>
@@ -1182,7 +1222,9 @@
       <c r="H10" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="4"/>
+      <c r="I10" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J10" s="4" t="s">
         <v>18</v>
       </c>
@@ -1212,7 +1254,9 @@
       <c r="H11" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="I11" s="4"/>
+      <c r="I11" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="J11" s="4" t="s">
         <v>21</v>
       </c>
@@ -1242,7 +1286,9 @@
       <c r="H12" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="I12" s="4"/>
+      <c r="I12" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="J12" s="4" t="s">
         <v>23</v>
       </c>
@@ -1272,7 +1318,9 @@
       <c r="H13" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="I13" s="4"/>
+      <c r="I13" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="J13" s="4" t="s">
         <v>21</v>
       </c>
@@ -1300,7 +1348,9 @@
       <c r="H14" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="I14" s="4"/>
+      <c r="I14" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="J14" s="4" t="s">
         <v>18</v>
       </c>
@@ -1326,7 +1376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Testes de performance no relatorio concluídos. Falta a conclusão ainda hoje!!
</commit_message>
<xml_diff>
--- a/gesthiper.xlsx
+++ b/gesthiper.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\José Carlos\Desktop\2º Semestre\Laboratórios de Informática  III\C\LI3_GZT-master\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -278,7 +273,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -375,8 +370,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="113">
+  <cellStyleXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -527,119 +530,127 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="113">
-    <cellStyle name="Hiperligação" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="112" builtinId="9" hidden="1"/>
+  <cellStyles count="121">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -983,16 +994,16 @@
       <selection activeCell="H1" sqref="H1:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="5" width="21.625" customWidth="1"/>
+    <col min="2" max="5" width="21.6640625" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
-    <col min="7" max="7" width="21.625" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" customWidth="1"/>
     <col min="8" max="8" width="21.5" customWidth="1"/>
-    <col min="9" max="9" width="21.625" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" customWidth="1"/>
     <col min="10" max="10" width="27" customWidth="1"/>
     <col min="11" max="11" width="27.5" customWidth="1"/>
-    <col min="12" max="12" width="26.875" customWidth="1"/>
+    <col min="12" max="12" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1466,13 +1477,13 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="12.625" customWidth="1"/>
-    <col min="4" max="4" width="21.125" customWidth="1"/>
-    <col min="5" max="5" width="12.375" customWidth="1"/>
-    <col min="6" max="6" width="16.625" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1686,12 +1697,12 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1743,11 +1754,11 @@
       <c r="B4" s="13">
         <v>57.01</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4">
+        <v>59.42</v>
+      </c>
+      <c r="D4" s="14">
         <v>63.62</v>
-      </c>
-      <c r="D4" s="14">
-        <v>59.42</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1904,7 +1915,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>